<commit_message>
feat: Implemented data grouping structure to enhance data processing and synchronization between frontend and backend.
</commit_message>
<xml_diff>
--- a/backend/uploads/1. Current Shunt_sample.xlsx
+++ b/backend/uploads/1. Current Shunt_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a516e\Jupyter Notebooks\magang\DCC\lab kelistrikan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\12. Digital Transformation Metrology\CABUREK 2024 - 2025\Contoh Sertifikat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53ED32D-A2DD-445A-ABF2-DEDFDBECA4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6102C56-58C6-4717-B3B0-6DBAE634EACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="720" yWindow="720" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{43E7CF36-0312-49AC-81BF-6DD2F08AA4DF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{43E7CF36-0312-49AC-81BF-6DD2F08AA4DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Eva" sheetId="2" r:id="rId1"/>
@@ -20,17 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1245,6 +1234,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1254,83 +1279,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="7" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="7" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1357,9 +1346,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1397,7 +1386,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1503,7 +1492,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1645,7 +1634,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1659,64 +1648,64 @@
       <selection activeCell="BA33" sqref="BA33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="5.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" customWidth="1"/>
-    <col min="11" max="11" width="6.21875" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" customWidth="1"/>
-    <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.44140625" customWidth="1"/>
-    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.44140625" customWidth="1"/>
-    <col min="19" max="19" width="11.44140625" customWidth="1"/>
-    <col min="20" max="20" width="6.88671875" customWidth="1"/>
-    <col min="21" max="21" width="11.88671875" customWidth="1"/>
-    <col min="22" max="22" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="5.453125" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="9" max="9" width="6.6328125" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" customWidth="1"/>
+    <col min="11" max="11" width="6.26953125" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.453125" customWidth="1"/>
+    <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.453125" customWidth="1"/>
+    <col min="19" max="19" width="11.453125" customWidth="1"/>
+    <col min="20" max="20" width="6.90625" customWidth="1"/>
+    <col min="21" max="21" width="11.90625" customWidth="1"/>
+    <col min="22" max="22" width="7.08984375" customWidth="1"/>
     <col min="23" max="23" width="12" customWidth="1"/>
-    <col min="24" max="24" width="7.21875" customWidth="1"/>
-    <col min="25" max="25" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.1796875" customWidth="1"/>
+    <col min="25" max="25" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10" customWidth="1"/>
-    <col min="28" max="28" width="6.77734375" customWidth="1"/>
+    <col min="28" max="28" width="6.81640625" customWidth="1"/>
     <col min="30" max="30" width="11" customWidth="1"/>
-    <col min="31" max="31" width="6.44140625" customWidth="1"/>
-    <col min="32" max="32" width="10.88671875" style="44" customWidth="1"/>
-    <col min="33" max="33" width="5.44140625" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.77734375" customWidth="1"/>
-    <col min="37" max="37" width="6.77734375" customWidth="1"/>
-    <col min="42" max="42" width="10.33203125" customWidth="1"/>
-    <col min="43" max="43" width="7.44140625" customWidth="1"/>
-    <col min="45" max="45" width="10.77734375" customWidth="1"/>
-    <col min="46" max="46" width="5.77734375" customWidth="1"/>
-    <col min="47" max="47" width="10.6640625" customWidth="1"/>
+    <col min="31" max="31" width="6.453125" customWidth="1"/>
+    <col min="32" max="32" width="10.90625" style="44" customWidth="1"/>
+    <col min="33" max="33" width="5.453125" customWidth="1"/>
+    <col min="34" max="34" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.81640625" customWidth="1"/>
+    <col min="37" max="37" width="6.7265625" customWidth="1"/>
+    <col min="42" max="42" width="10.36328125" customWidth="1"/>
+    <col min="43" max="43" width="7.453125" customWidth="1"/>
+    <col min="45" max="45" width="10.7265625" customWidth="1"/>
+    <col min="46" max="46" width="5.7265625" customWidth="1"/>
+    <col min="47" max="47" width="10.6328125" customWidth="1"/>
     <col min="48" max="48" width="7" customWidth="1"/>
-    <col min="49" max="49" width="9.77734375" customWidth="1"/>
-    <col min="50" max="50" width="6.5546875" customWidth="1"/>
-    <col min="51" max="51" width="10.77734375" customWidth="1"/>
-    <col min="52" max="52" width="6.5546875" customWidth="1"/>
-    <col min="53" max="53" width="9.21875" customWidth="1"/>
-    <col min="54" max="54" width="7.33203125" customWidth="1"/>
-    <col min="63" max="63" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10.44140625" customWidth="1"/>
-    <col min="68" max="68" width="13.6640625" customWidth="1"/>
-    <col min="69" max="69" width="10.109375" customWidth="1"/>
-    <col min="70" max="70" width="8.109375" customWidth="1"/>
+    <col min="49" max="49" width="9.81640625" customWidth="1"/>
+    <col min="50" max="50" width="6.54296875" customWidth="1"/>
+    <col min="51" max="51" width="10.81640625" customWidth="1"/>
+    <col min="52" max="52" width="6.54296875" customWidth="1"/>
+    <col min="53" max="53" width="9.1796875" customWidth="1"/>
+    <col min="54" max="54" width="7.36328125" customWidth="1"/>
+    <col min="63" max="63" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.453125" customWidth="1"/>
+    <col min="68" max="68" width="13.6328125" customWidth="1"/>
+    <col min="69" max="69" width="10.08984375" customWidth="1"/>
+    <col min="70" max="70" width="8.08984375" customWidth="1"/>
     <col min="72" max="72" width="10" customWidth="1"/>
-    <col min="73" max="73" width="8.109375" customWidth="1"/>
+    <col min="73" max="73" width="8.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:73" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="40" t="s">
         <v>50</v>
       </c>
@@ -1725,101 +1714,101 @@
       <c r="D1" s="41"/>
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
-      <c r="O1" s="69" t="s">
+      <c r="O1" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="71"/>
-      <c r="AD1" s="69" t="s">
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="83"/>
+      <c r="AD1" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="70"/>
-      <c r="AL1" s="70"/>
-      <c r="AM1" s="70"/>
-      <c r="AN1" s="70"/>
-      <c r="AO1" s="70"/>
-      <c r="AP1" s="70"/>
-      <c r="AQ1" s="71"/>
-      <c r="AS1" s="72" t="s">
+      <c r="AE1" s="82"/>
+      <c r="AF1" s="82"/>
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="82"/>
+      <c r="AI1" s="82"/>
+      <c r="AJ1" s="82"/>
+      <c r="AK1" s="82"/>
+      <c r="AL1" s="82"/>
+      <c r="AM1" s="82"/>
+      <c r="AN1" s="82"/>
+      <c r="AO1" s="82"/>
+      <c r="AP1" s="82"/>
+      <c r="AQ1" s="83"/>
+      <c r="AS1" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="AT1" s="72"/>
-      <c r="AU1" s="72"/>
-      <c r="AV1" s="72"/>
-      <c r="AW1" s="72"/>
-      <c r="AX1" s="72"/>
-      <c r="AY1" s="72"/>
-      <c r="AZ1" s="72"/>
-      <c r="BA1" s="72"/>
-      <c r="BB1" s="72"/>
-    </row>
-    <row r="2" spans="1:73" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="73" t="s">
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="78"/>
+      <c r="BA1" s="78"/>
+      <c r="BB1" s="78"/>
+    </row>
+    <row r="2" spans="1:73" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="76" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="77"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="42"/>
       <c r="G2" s="43"/>
-      <c r="H2" s="80" t="s">
+      <c r="H2" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80" t="s">
+      <c r="I2" s="69"/>
+      <c r="J2" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80" t="s">
+      <c r="K2" s="69"/>
+      <c r="L2" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="80"/>
-      <c r="O2" s="81" t="s">
+      <c r="M2" s="69"/>
+      <c r="O2" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="81" t="s">
+      <c r="P2" s="80"/>
+      <c r="Q2" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="R2" s="82"/>
-      <c r="S2" s="81" t="s">
+      <c r="R2" s="80"/>
+      <c r="S2" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="82"/>
-      <c r="U2" s="81" t="s">
+      <c r="T2" s="80"/>
+      <c r="U2" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="V2" s="82"/>
-      <c r="W2" s="81" t="s">
+      <c r="V2" s="80"/>
+      <c r="W2" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="X2" s="82"/>
-      <c r="Y2" s="81" t="s">
+      <c r="X2" s="80"/>
+      <c r="Y2" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="Z2" s="82"/>
+      <c r="Z2" s="80"/>
       <c r="AA2" s="65" t="s">
         <v>66</v>
       </c>
@@ -1864,26 +1853,26 @@
         <v>74</v>
       </c>
       <c r="AX2" s="66"/>
-      <c r="AY2" s="80" t="s">
+      <c r="AY2" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="AZ2" s="80"/>
+      <c r="AZ2" s="69"/>
       <c r="BA2" s="65" t="s">
         <v>66</v>
       </c>
       <c r="BB2" s="66"/>
-      <c r="BD2" s="80" t="s">
+      <c r="BD2" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="BE2" s="80"/>
-      <c r="BF2" s="80" t="s">
+      <c r="BE2" s="69"/>
+      <c r="BF2" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="BG2" s="80"/>
-      <c r="BH2" s="80" t="s">
+      <c r="BG2" s="69"/>
+      <c r="BH2" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="BI2" s="80"/>
+      <c r="BI2" s="69"/>
       <c r="BK2" s="65" t="s">
         <v>79</v>
       </c>
@@ -1896,32 +1885,32 @@
         <v>79</v>
       </c>
       <c r="BP2" s="66"/>
-      <c r="BQ2" s="80" t="s">
+      <c r="BQ2" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="BR2" s="80"/>
-      <c r="BS2" s="80" t="s">
+      <c r="BR2" s="69"/>
+      <c r="BS2" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="BT2" s="80" t="s">
+      <c r="BT2" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="BU2" s="80"/>
-    </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
-      <c r="A3" s="74"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="79"/>
+      <c r="BU2" s="69"/>
+    </row>
+    <row r="3" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A3" s="85"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="42"/>
       <c r="G3" s="43"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
       <c r="O3" s="67"/>
       <c r="P3" s="68"/>
       <c r="Q3" s="67"/>
@@ -1956,29 +1945,29 @@
       <c r="AV3" s="68"/>
       <c r="AW3" s="67"/>
       <c r="AX3" s="68"/>
-      <c r="AY3" s="80"/>
-      <c r="AZ3" s="80"/>
+      <c r="AY3" s="69"/>
+      <c r="AZ3" s="69"/>
       <c r="BA3" s="67"/>
       <c r="BB3" s="68"/>
-      <c r="BD3" s="80"/>
-      <c r="BE3" s="80"/>
-      <c r="BF3" s="80"/>
-      <c r="BG3" s="80"/>
-      <c r="BH3" s="80"/>
-      <c r="BI3" s="80"/>
+      <c r="BD3" s="69"/>
+      <c r="BE3" s="69"/>
+      <c r="BF3" s="69"/>
+      <c r="BG3" s="69"/>
+      <c r="BH3" s="69"/>
+      <c r="BI3" s="69"/>
       <c r="BK3" s="67"/>
       <c r="BL3" s="68"/>
       <c r="BM3" s="67"/>
       <c r="BN3" s="68"/>
       <c r="BO3" s="67"/>
       <c r="BP3" s="68"/>
-      <c r="BQ3" s="80"/>
-      <c r="BR3" s="80"/>
-      <c r="BS3" s="80"/>
-      <c r="BT3" s="80"/>
-      <c r="BU3" s="80"/>
-    </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="BQ3" s="69"/>
+      <c r="BR3" s="69"/>
+      <c r="BS3" s="69"/>
+      <c r="BT3" s="69"/>
+      <c r="BU3" s="69"/>
+    </row>
+    <row r="4" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A4" s="44" t="s">
         <v>83</v>
       </c>
@@ -2078,10 +2067,10 @@
       <c r="AK4" t="s">
         <v>85</v>
       </c>
-      <c r="AL4" s="83" t="s">
+      <c r="AL4" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="AM4" s="83"/>
+      <c r="AM4" s="76"/>
       <c r="AN4">
         <v>1E-3</v>
       </c>
@@ -2177,7 +2166,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A5" s="44" t="s">
         <v>91</v>
       </c>
@@ -2201,8 +2190,8 @@
       <c r="AD5" s="47"/>
       <c r="AE5" s="47"/>
       <c r="AF5" s="51"/>
-      <c r="AL5" s="84"/>
-      <c r="AM5" s="84"/>
+      <c r="AL5" s="77"/>
+      <c r="AM5" s="77"/>
       <c r="AP5" s="58"/>
       <c r="AS5" s="47"/>
       <c r="AU5" s="47"/>
@@ -2214,7 +2203,7 @@
       <c r="BO5" s="55"/>
       <c r="BQ5" s="57"/>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A6" s="44" t="s">
         <v>83</v>
       </c>
@@ -2314,8 +2303,8 @@
       <c r="AK6" t="s">
         <v>85</v>
       </c>
-      <c r="AL6" s="84"/>
-      <c r="AM6" s="84"/>
+      <c r="AL6" s="77"/>
+      <c r="AM6" s="77"/>
       <c r="AN6">
         <v>1E-3</v>
       </c>
@@ -2411,7 +2400,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A7" s="44" t="s">
         <v>91</v>
       </c>
@@ -2436,8 +2425,8 @@
       <c r="AD7" s="47"/>
       <c r="AE7" s="47"/>
       <c r="AF7" s="51"/>
-      <c r="AL7" s="84"/>
-      <c r="AM7" s="84"/>
+      <c r="AL7" s="77"/>
+      <c r="AM7" s="77"/>
       <c r="AP7" s="58"/>
       <c r="AS7" s="47"/>
       <c r="AU7" s="47"/>
@@ -2449,7 +2438,7 @@
       <c r="BO7" s="55"/>
       <c r="BQ7" s="57"/>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A8" s="44" t="s">
         <v>83</v>
       </c>
@@ -2549,8 +2538,8 @@
       <c r="AK8" t="s">
         <v>85</v>
       </c>
-      <c r="AL8" s="84"/>
-      <c r="AM8" s="84"/>
+      <c r="AL8" s="77"/>
+      <c r="AM8" s="77"/>
       <c r="AN8">
         <v>1E-3</v>
       </c>
@@ -2646,7 +2635,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A9" s="44" t="s">
         <v>91</v>
       </c>
@@ -2671,8 +2660,8 @@
       <c r="AD9" s="47"/>
       <c r="AE9" s="47"/>
       <c r="AF9" s="51"/>
-      <c r="AL9" s="84"/>
-      <c r="AM9" s="84"/>
+      <c r="AL9" s="77"/>
+      <c r="AM9" s="77"/>
       <c r="AP9" s="58"/>
       <c r="AS9" s="47"/>
       <c r="AU9" s="47"/>
@@ -2684,7 +2673,7 @@
       <c r="BO9" s="55"/>
       <c r="BQ9" s="57"/>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A10" s="44" t="s">
         <v>83</v>
       </c>
@@ -2784,8 +2773,8 @@
       <c r="AK10" t="s">
         <v>85</v>
       </c>
-      <c r="AL10" s="84"/>
-      <c r="AM10" s="84"/>
+      <c r="AL10" s="77"/>
+      <c r="AM10" s="77"/>
       <c r="AN10">
         <v>1E-3</v>
       </c>
@@ -2881,7 +2870,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A11" s="44" t="s">
         <v>91</v>
       </c>
@@ -2906,8 +2895,8 @@
       <c r="AD11" s="47"/>
       <c r="AE11" s="47"/>
       <c r="AF11" s="51"/>
-      <c r="AL11" s="84"/>
-      <c r="AM11" s="84"/>
+      <c r="AL11" s="77"/>
+      <c r="AM11" s="77"/>
       <c r="AP11" s="58"/>
       <c r="AS11" s="47"/>
       <c r="AU11" s="47"/>
@@ -2919,7 +2908,7 @@
       <c r="BO11" s="55"/>
       <c r="BQ11" s="57"/>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A12" s="44" t="s">
         <v>83</v>
       </c>
@@ -3019,8 +3008,8 @@
       <c r="AK12" t="s">
         <v>85</v>
       </c>
-      <c r="AL12" s="84"/>
-      <c r="AM12" s="84"/>
+      <c r="AL12" s="77"/>
+      <c r="AM12" s="77"/>
       <c r="AN12">
         <v>1E-3</v>
       </c>
@@ -3116,7 +3105,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A13" s="44" t="s">
         <v>91</v>
       </c>
@@ -3143,8 +3132,8 @@
       <c r="AF13" s="51"/>
       <c r="AH13" s="52"/>
       <c r="AI13" s="52"/>
-      <c r="AL13" s="84"/>
-      <c r="AM13" s="84"/>
+      <c r="AL13" s="77"/>
+      <c r="AM13" s="77"/>
       <c r="AP13" s="58"/>
       <c r="AS13" s="47"/>
       <c r="AU13" s="47"/>
@@ -3156,7 +3145,7 @@
       <c r="BO13" s="55"/>
       <c r="BQ13" s="57"/>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A14" s="44" t="s">
         <v>83</v>
       </c>
@@ -3256,8 +3245,8 @@
       <c r="AK14" t="s">
         <v>85</v>
       </c>
-      <c r="AL14" s="84"/>
-      <c r="AM14" s="84"/>
+      <c r="AL14" s="77"/>
+      <c r="AM14" s="77"/>
       <c r="AN14">
         <v>1E-3</v>
       </c>
@@ -3353,7 +3342,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
         <v>91</v>
       </c>
@@ -3380,8 +3369,8 @@
       <c r="AF15" s="51"/>
       <c r="AH15" s="52"/>
       <c r="AI15" s="52"/>
-      <c r="AL15" s="84"/>
-      <c r="AM15" s="84"/>
+      <c r="AL15" s="77"/>
+      <c r="AM15" s="77"/>
       <c r="AP15" s="58"/>
       <c r="AS15" s="47"/>
       <c r="AU15" s="47"/>
@@ -3393,7 +3382,7 @@
       <c r="BO15" s="55"/>
       <c r="BQ15" s="57"/>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A16" s="44" t="s">
         <v>83</v>
       </c>
@@ -3493,8 +3482,8 @@
       <c r="AK16" t="s">
         <v>85</v>
       </c>
-      <c r="AL16" s="84"/>
-      <c r="AM16" s="84"/>
+      <c r="AL16" s="77"/>
+      <c r="AM16" s="77"/>
       <c r="AN16">
         <v>1E-3</v>
       </c>
@@ -3590,7 +3579,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A17" s="44" t="s">
         <v>91</v>
       </c>
@@ -3615,8 +3604,8 @@
       <c r="AD17" s="47"/>
       <c r="AE17" s="47"/>
       <c r="AF17" s="51"/>
-      <c r="AL17" s="84"/>
-      <c r="AM17" s="84"/>
+      <c r="AL17" s="77"/>
+      <c r="AM17" s="77"/>
       <c r="AP17" s="58"/>
       <c r="AS17" s="47"/>
       <c r="AU17" s="47"/>
@@ -3628,7 +3617,7 @@
       <c r="BO17" s="55"/>
       <c r="BQ17" s="57"/>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A18" s="44" t="s">
         <v>83</v>
       </c>
@@ -3728,8 +3717,8 @@
       <c r="AK18" t="s">
         <v>85</v>
       </c>
-      <c r="AL18" s="84"/>
-      <c r="AM18" s="84"/>
+      <c r="AL18" s="77"/>
+      <c r="AM18" s="77"/>
       <c r="AN18">
         <v>1E-3</v>
       </c>
@@ -3825,7 +3814,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A19" s="44" t="s">
         <v>91</v>
       </c>
@@ -3845,7 +3834,7 @@
       <c r="AD19" s="47"/>
       <c r="AE19" s="47"/>
     </row>
-    <row r="22" spans="1:73" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:73" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="40" t="s">
         <v>93</v>
       </c>
@@ -3853,91 +3842,91 @@
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
-      <c r="O22" s="72" t="s">
+      <c r="O22" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="P22" s="72"/>
-      <c r="Q22" s="72"/>
-      <c r="R22" s="72"/>
-      <c r="S22" s="72"/>
-      <c r="T22" s="72"/>
-      <c r="U22" s="72"/>
-      <c r="V22" s="72"/>
-      <c r="W22" s="72"/>
-      <c r="X22" s="72"/>
-      <c r="AD22" s="72" t="s">
+      <c r="P22" s="78"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78"/>
+      <c r="S22" s="78"/>
+      <c r="T22" s="78"/>
+      <c r="U22" s="78"/>
+      <c r="V22" s="78"/>
+      <c r="W22" s="78"/>
+      <c r="X22" s="78"/>
+      <c r="AD22" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="AE22" s="72"/>
-      <c r="AF22" s="72"/>
-      <c r="AG22" s="72"/>
-      <c r="AH22" s="72"/>
-      <c r="AI22" s="72"/>
-      <c r="AJ22" s="72"/>
-      <c r="AK22" s="72"/>
-    </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.3">
-      <c r="A23" s="85"/>
-      <c r="B23" s="75" t="s">
+      <c r="AE22" s="78"/>
+      <c r="AF22" s="78"/>
+      <c r="AG22" s="78"/>
+      <c r="AH22" s="78"/>
+      <c r="AI22" s="78"/>
+      <c r="AJ22" s="78"/>
+      <c r="AK22" s="78"/>
+    </row>
+    <row r="23" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A23" s="70"/>
+      <c r="B23" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="75"/>
-      <c r="D23" s="80" t="s">
+      <c r="C23" s="71"/>
+      <c r="D23" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="80"/>
-      <c r="F23" s="76" t="s">
+      <c r="E23" s="69"/>
+      <c r="F23" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="77"/>
-      <c r="H23" s="80" t="s">
+      <c r="G23" s="73"/>
+      <c r="H23" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80" t="s">
+      <c r="I23" s="69"/>
+      <c r="J23" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="K23" s="80"/>
-      <c r="L23" s="80" t="s">
+      <c r="K23" s="69"/>
+      <c r="L23" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="M23" s="80"/>
-      <c r="O23" s="80" t="s">
+      <c r="M23" s="69"/>
+      <c r="O23" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="P23" s="80"/>
-      <c r="Q23" s="80" t="s">
+      <c r="P23" s="69"/>
+      <c r="Q23" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="R23" s="80"/>
-      <c r="S23" s="80" t="s">
+      <c r="R23" s="69"/>
+      <c r="S23" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="T23" s="80"/>
-      <c r="U23" s="80" t="s">
+      <c r="T23" s="69"/>
+      <c r="U23" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="V23" s="80"/>
-      <c r="W23" s="80" t="s">
+      <c r="V23" s="69"/>
+      <c r="W23" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="X23" s="80"/>
-      <c r="AD23" s="80" t="s">
+      <c r="X23" s="69"/>
+      <c r="AD23" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="AE23" s="80"/>
-      <c r="AF23" s="80" t="s">
+      <c r="AE23" s="69"/>
+      <c r="AF23" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="AG23" s="80"/>
-      <c r="AH23" s="80" t="s">
+      <c r="AG23" s="69"/>
+      <c r="AH23" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="AI23" s="80"/>
-      <c r="AJ23" s="80" t="s">
+      <c r="AI23" s="69"/>
+      <c r="AJ23" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="AK23" s="80"/>
+      <c r="AK23" s="69"/>
       <c r="AN23" s="65" t="s">
         <v>77</v>
       </c>
@@ -3954,51 +3943,51 @@
         <v>108</v>
       </c>
       <c r="AV23" s="66"/>
-      <c r="AW23" s="80" t="s">
+      <c r="AW23" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="AX23" s="80"/>
-      <c r="AY23" s="80" t="s">
+      <c r="AX23" s="69"/>
+      <c r="AY23" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="BA23" s="80" t="s">
+      <c r="BA23" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="BB23" s="80"/>
+      <c r="BB23" s="69"/>
       <c r="BC23" s="59"/>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.3">
-      <c r="A24" s="85"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
-      <c r="O24" s="80"/>
-      <c r="P24" s="80"/>
-      <c r="Q24" s="80"/>
-      <c r="R24" s="80"/>
-      <c r="S24" s="80"/>
-      <c r="T24" s="80"/>
-      <c r="U24" s="80"/>
-      <c r="V24" s="80"/>
-      <c r="W24" s="80"/>
-      <c r="X24" s="80"/>
-      <c r="AD24" s="80"/>
-      <c r="AE24" s="80"/>
-      <c r="AF24" s="80"/>
-      <c r="AG24" s="80"/>
-      <c r="AH24" s="80"/>
-      <c r="AI24" s="80"/>
-      <c r="AJ24" s="80"/>
-      <c r="AK24" s="80"/>
+    <row r="24" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A24" s="70"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="69"/>
+      <c r="Q24" s="69"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="69"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="69"/>
+      <c r="V24" s="69"/>
+      <c r="W24" s="69"/>
+      <c r="X24" s="69"/>
+      <c r="AD24" s="69"/>
+      <c r="AE24" s="69"/>
+      <c r="AF24" s="69"/>
+      <c r="AG24" s="69"/>
+      <c r="AH24" s="69"/>
+      <c r="AI24" s="69"/>
+      <c r="AJ24" s="69"/>
+      <c r="AK24" s="69"/>
       <c r="AN24" s="67"/>
       <c r="AO24" s="68"/>
       <c r="AP24" s="67"/>
@@ -4007,14 +3996,14 @@
       <c r="AT24" s="68"/>
       <c r="AU24" s="67"/>
       <c r="AV24" s="68"/>
-      <c r="AW24" s="80"/>
-      <c r="AX24" s="80"/>
-      <c r="AY24" s="80"/>
-      <c r="BA24" s="80"/>
-      <c r="BB24" s="80"/>
+      <c r="AW24" s="69"/>
+      <c r="AX24" s="69"/>
+      <c r="AY24" s="69"/>
+      <c r="BA24" s="69"/>
+      <c r="BB24" s="69"/>
       <c r="BC24" s="59"/>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>3</v>
       </c>
@@ -4146,7 +4135,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>3</v>
       </c>
@@ -4278,7 +4267,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>3</v>
       </c>
@@ -4410,7 +4399,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>15</v>
       </c>
@@ -4542,7 +4531,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>15</v>
       </c>
@@ -4674,7 +4663,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>15</v>
       </c>
@@ -4806,7 +4795,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>20</v>
       </c>
@@ -4938,7 +4927,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>20</v>
       </c>
@@ -5070,7 +5059,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>20</v>
       </c>
@@ -5202,35 +5191,38 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:54" x14ac:dyDescent="0.35">
       <c r="AS34" s="47"/>
       <c r="AU34" s="48"/>
       <c r="AY34" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="AS23:AT24"/>
-    <mergeCell ref="AU23:AV24"/>
-    <mergeCell ref="AW23:AX24"/>
-    <mergeCell ref="AY23:AY24"/>
-    <mergeCell ref="BA23:BB24"/>
-    <mergeCell ref="AP23:AQ24"/>
-    <mergeCell ref="L23:M24"/>
-    <mergeCell ref="O23:P24"/>
-    <mergeCell ref="Q23:R24"/>
-    <mergeCell ref="S23:T24"/>
-    <mergeCell ref="U23:V24"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="AD23:AE24"/>
-    <mergeCell ref="AF23:AG24"/>
-    <mergeCell ref="AH23:AI24"/>
-    <mergeCell ref="AJ23:AK24"/>
-    <mergeCell ref="AN23:AO24"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="D23:E24"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="AA2:AB3"/>
+    <mergeCell ref="O1:AB1"/>
+    <mergeCell ref="AD1:AQ1"/>
+    <mergeCell ref="AS1:BB1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="J2:K3"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="O2:P3"/>
+    <mergeCell ref="Q2:R3"/>
+    <mergeCell ref="S2:T3"/>
+    <mergeCell ref="U2:V3"/>
+    <mergeCell ref="W2:X3"/>
+    <mergeCell ref="Y2:Z3"/>
+    <mergeCell ref="AW2:AX3"/>
+    <mergeCell ref="AY2:AZ3"/>
+    <mergeCell ref="BA2:BB3"/>
+    <mergeCell ref="AD2:AE3"/>
+    <mergeCell ref="AF2:AG3"/>
+    <mergeCell ref="AH2:AI3"/>
+    <mergeCell ref="AJ2:AK3"/>
+    <mergeCell ref="AL2:AM3"/>
+    <mergeCell ref="AN2:AO3"/>
     <mergeCell ref="J23:K24"/>
     <mergeCell ref="BQ2:BR3"/>
     <mergeCell ref="BS2:BS3"/>
@@ -5247,31 +5239,28 @@
     <mergeCell ref="AP2:AQ3"/>
     <mergeCell ref="AS2:AT3"/>
     <mergeCell ref="AU2:AV3"/>
-    <mergeCell ref="AW2:AX3"/>
-    <mergeCell ref="AY2:AZ3"/>
-    <mergeCell ref="BA2:BB3"/>
-    <mergeCell ref="AD2:AE3"/>
-    <mergeCell ref="AF2:AG3"/>
-    <mergeCell ref="AH2:AI3"/>
-    <mergeCell ref="AJ2:AK3"/>
-    <mergeCell ref="AL2:AM3"/>
-    <mergeCell ref="AN2:AO3"/>
-    <mergeCell ref="AA2:AB3"/>
-    <mergeCell ref="O1:AB1"/>
-    <mergeCell ref="AD1:AQ1"/>
-    <mergeCell ref="AS1:BB1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="J2:K3"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="O2:P3"/>
-    <mergeCell ref="Q2:R3"/>
-    <mergeCell ref="S2:T3"/>
-    <mergeCell ref="U2:V3"/>
-    <mergeCell ref="W2:X3"/>
-    <mergeCell ref="Y2:Z3"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:C24"/>
+    <mergeCell ref="D23:E24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="AP23:AQ24"/>
+    <mergeCell ref="L23:M24"/>
+    <mergeCell ref="O23:P24"/>
+    <mergeCell ref="Q23:R24"/>
+    <mergeCell ref="S23:T24"/>
+    <mergeCell ref="U23:V24"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="AD23:AE24"/>
+    <mergeCell ref="AF23:AG24"/>
+    <mergeCell ref="AH23:AI24"/>
+    <mergeCell ref="AJ23:AK24"/>
+    <mergeCell ref="AN23:AO24"/>
+    <mergeCell ref="AS23:AT24"/>
+    <mergeCell ref="AU23:AV24"/>
+    <mergeCell ref="AW23:AX24"/>
+    <mergeCell ref="AY23:AY24"/>
+    <mergeCell ref="BA23:BB24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5281,132 +5270,132 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA858041-4D01-4E9F-9819-708CBB21ED46}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.21875" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="1.1796875" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" customWidth="1"/>
+    <col min="3" max="3" width="3.36328125" customWidth="1"/>
     <col min="4" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" customWidth="1"/>
-    <col min="12" max="12" width="10.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" customWidth="1"/>
+    <col min="10" max="10" width="11.08984375" customWidth="1"/>
+    <col min="11" max="11" width="7.90625" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="87" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="88" t="s">
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="86" t="s">
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87" t="s">
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="87" t="s">
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="86" t="s">
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="88" t="s">
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="86" t="s">
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="87" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -5419,7 +5408,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -5432,23 +5421,23 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="92" t="s">
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.35">
+      <c r="A9" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="87"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -5461,59 +5450,59 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="96" t="s">
+    <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="96"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="93"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="97" t="s">
+    <row r="12" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="88" t="s">
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="88"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="88"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="97" t="s">
+      <c r="J12" s="95"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="95"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="88" t="s">
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J13" s="95"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -5526,7 +5515,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -5539,7 +5528,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="2"/>
       <c r="D16" s="5" t="s">
         <v>112</v>
@@ -5553,47 +5542,47 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="89" t="s">
+      <c r="D17" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89" t="s">
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="89"/>
-      <c r="J17" s="90" t="s">
+      <c r="I17" s="88"/>
+      <c r="J17" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="90"/>
+      <c r="K17" s="89"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="93" t="s">
+      <c r="D18" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93" t="s">
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="93"/>
-      <c r="J18" s="94" t="s">
+      <c r="I18" s="90"/>
+      <c r="J18" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="94"/>
+      <c r="K18" s="91"/>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -5623,7 +5612,7 @@
       </c>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="E20" s="61">
@@ -5652,7 +5641,7 @@
       </c>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="E21" s="61">
@@ -5681,7 +5670,7 @@
       </c>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="E22" s="61">
@@ -5710,7 +5699,7 @@
       </c>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="E23" s="61">
@@ -5739,7 +5728,7 @@
       </c>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="E24" s="61">
@@ -5768,7 +5757,7 @@
       </c>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="E25" s="61">
@@ -5797,7 +5786,7 @@
       </c>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="E26" s="61">
@@ -5826,7 +5815,7 @@
       </c>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -5839,7 +5828,7 @@
       <c r="K27" s="16"/>
       <c r="L27" s="13"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="14"/>
@@ -5851,7 +5840,7 @@
       <c r="K28" s="16"/>
       <c r="L28" s="13"/>
     </row>
-    <row r="29" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="5" t="s">
@@ -5866,46 +5855,46 @@
       <c r="K29" s="2"/>
       <c r="L29" s="17"/>
     </row>
-    <row r="30" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.35">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="89" t="s">
+      <c r="D30" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89" t="s">
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
+      <c r="H30" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="I30" s="89"/>
-      <c r="J30" s="90" t="s">
+      <c r="I30" s="88"/>
+      <c r="J30" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="K30" s="90"/>
+      <c r="K30" s="89"/>
       <c r="L30" s="17"/>
     </row>
-    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
-      <c r="D31" s="93" t="s">
+      <c r="D31" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93" t="s">
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
+      <c r="H31" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="93"/>
-      <c r="J31" s="94" t="s">
+      <c r="I31" s="90"/>
+      <c r="J31" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="K31" s="94"/>
+      <c r="K31" s="91"/>
       <c r="L31" s="17"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -5943,7 +5932,7 @@
       </c>
       <c r="L32" s="17"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -5981,7 +5970,7 @@
       </c>
       <c r="L33" s="17"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -6019,7 +6008,7 @@
       </c>
       <c r="L34" s="17"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -6057,7 +6046,7 @@
       </c>
       <c r="L35" s="17"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -6095,7 +6084,7 @@
       </c>
       <c r="L36" s="17"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -6133,7 +6122,7 @@
       </c>
       <c r="L37" s="17"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -6171,7 +6160,7 @@
       </c>
       <c r="L38" s="17"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -6209,7 +6198,7 @@
       </c>
       <c r="L39" s="17"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -6247,7 +6236,7 @@
       </c>
       <c r="L40" s="19"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -6261,7 +6250,7 @@
       <c r="K41" s="16"/>
       <c r="L41" s="19"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -6275,12 +6264,12 @@
       <c r="K42" s="16"/>
       <c r="L42" s="19"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="95" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B43" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="95"/>
-      <c r="D43" s="95"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
@@ -6290,7 +6279,7 @@
       <c r="K43" s="23"/>
       <c r="L43" s="23"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -6308,7 +6297,7 @@
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B45" s="24" t="s">
         <v>19</v>
       </c>
@@ -6323,7 +6312,7 @@
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B46" s="25" t="s">
         <v>20</v>
       </c>
@@ -6338,7 +6327,7 @@
       <c r="K46" s="23"/>
       <c r="L46" s="23"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -6356,7 +6345,7 @@
       <c r="K47" s="23"/>
       <c r="L47" s="23"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B48" s="24" t="s">
         <v>31</v>
       </c>
@@ -6371,7 +6360,7 @@
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B49" s="25" t="s">
         <v>22</v>
       </c>
@@ -6386,7 +6375,7 @@
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B50" s="25" t="s">
         <v>23</v>
       </c>
@@ -6401,7 +6390,7 @@
       <c r="K50" s="23"/>
       <c r="L50" s="23"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -6419,7 +6408,7 @@
       <c r="K51" s="23"/>
       <c r="L51" s="23"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B52" s="24" t="s">
         <v>25</v>
       </c>
@@ -6434,7 +6423,7 @@
       <c r="K52" s="23"/>
       <c r="L52" s="23"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B53" s="24" t="s">
         <v>32</v>
       </c>
@@ -6449,7 +6438,7 @@
       <c r="K53" s="23"/>
       <c r="L53" s="23"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B54" s="25" t="s">
         <v>26</v>
       </c>
@@ -6464,7 +6453,7 @@
       <c r="K54" s="23"/>
       <c r="L54" s="23"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B55" s="25" t="s">
         <v>27</v>
       </c>
@@ -6479,7 +6468,7 @@
       <c r="K55" s="23"/>
       <c r="L55" s="23"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="28" t="s">
         <v>17</v>
       </c>
@@ -6497,7 +6486,7 @@
       <c r="K56" s="30"/>
       <c r="L56" s="30"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="28"/>
       <c r="B57" s="24" t="s">
         <v>33</v>
@@ -6513,7 +6502,7 @@
       <c r="K57" s="30"/>
       <c r="L57" s="30"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="28"/>
       <c r="B58" s="25" t="s">
         <v>29</v>
@@ -6529,7 +6518,7 @@
       <c r="K58" s="30"/>
       <c r="L58" s="30"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="28"/>
       <c r="C59" s="29"/>
       <c r="D59" s="29"/>
@@ -6542,7 +6531,7 @@
       <c r="K59" s="30"/>
       <c r="L59" s="30"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B60" s="31"/>
       <c r="C60" s="27"/>
       <c r="D60" s="27"/>
@@ -6555,7 +6544,7 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
     </row>
-    <row r="61" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="38" t="s">
         <v>34</v>
       </c>
@@ -6572,7 +6561,7 @@
       <c r="K61" s="23"/>
       <c r="L61" s="23"/>
     </row>
-    <row r="62" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="38" t="s">
         <v>35</v>
       </c>
@@ -6589,7 +6578,7 @@
       <c r="K62" s="23"/>
       <c r="L62" s="23"/>
     </row>
-    <row r="63" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B63" s="35"/>
       <c r="C63" s="35"/>
       <c r="D63" s="35"/>
@@ -6604,7 +6593,7 @@
       <c r="K63" s="23"/>
       <c r="L63" s="23"/>
     </row>
-    <row r="64" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B64" s="35"/>
       <c r="C64" s="35"/>
       <c r="D64" s="35"/>
@@ -6619,7 +6608,7 @@
       <c r="K64" s="23"/>
       <c r="L64" s="23"/>
     </row>
-    <row r="65" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B65" s="35"/>
       <c r="C65" s="35"/>
       <c r="D65" s="35"/>
@@ -6634,7 +6623,7 @@
       <c r="K65" s="23"/>
       <c r="L65" s="23"/>
     </row>
-    <row r="66" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B66" s="35"/>
       <c r="C66" s="35"/>
       <c r="D66" s="35"/>
@@ -6647,23 +6636,23 @@
       <c r="K66" s="23"/>
       <c r="L66" s="23"/>
     </row>
-    <row r="67" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="91" t="s">
+    <row r="67" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="B67" s="91"/>
-      <c r="C67" s="91"/>
-      <c r="D67" s="91"/>
-      <c r="E67" s="91"/>
-      <c r="F67" s="91"/>
-      <c r="G67" s="91"/>
-      <c r="H67" s="91"/>
-      <c r="I67" s="91"/>
-      <c r="J67" s="91"/>
-      <c r="K67" s="91"/>
-      <c r="L67" s="91"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B67" s="86"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="86"/>
+      <c r="E67" s="86"/>
+      <c r="F67" s="86"/>
+      <c r="G67" s="86"/>
+      <c r="H67" s="86"/>
+      <c r="I67" s="86"/>
+      <c r="J67" s="86"/>
+      <c r="K67" s="86"/>
+      <c r="L67" s="86"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="E68" s="10"/>
@@ -6674,7 +6663,7 @@
       <c r="K68" s="37"/>
       <c r="L68" s="36"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="E69" s="10"/>
@@ -6685,7 +6674,7 @@
       <c r="K69" s="37"/>
       <c r="L69" s="36"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="E70" s="10"/>
@@ -6696,7 +6685,7 @@
       <c r="K70" s="37"/>
       <c r="L70" s="36"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="E71" s="10"/>
@@ -6709,6 +6698,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="I6:L6"/>
     <mergeCell ref="A67:L67"/>
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="H30:I30"/>
@@ -6725,22 +6730,6 @@
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="A13:H13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:L3"/>
   </mergeCells>
   <pageMargins left="0.98425196850393704" right="0.59055118110236227" top="1.9685039370078741" bottom="0.98425196850393704" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>